<commit_message>
added working jar file
</commit_message>
<xml_diff>
--- a/src/main/resources/Results.xlsx
+++ b/src/main/resources/Results.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielaarkind/Desktop/6 семестр/pudor/mortalkombatbLab52/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\IdeaProjects\mortalkombatLab5j\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F814BC09-BB69-FD4F-85B2-59E094602584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="14400"/>
   </bookViews>
   <sheets>
     <sheet name="Результаты ТОП 10" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>№</t>
   </si>
@@ -30,11 +29,14 @@
   <si>
     <t>Количество баллов</t>
   </si>
+  <si>
+    <t>Scorpion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,16 +381,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,6 +399,17 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>